<commit_message>
Added updated excel files and code
</commit_message>
<xml_diff>
--- a/transcendentDataset-AddedFeatures.xlsx
+++ b/transcendentDataset-AddedFeatures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Margie\Documents\University\University\IE_YOS4\SEM2\Lab Project ELEN4002\NNDev\Solvability-SourceCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A9D7D9-44B3-4AF4-BA27-6AD040CC2C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E75BA-F324-4F1A-8E5D-0AC9CC149A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{479CA36F-C05A-4624-8779-86DAF00DCCBB}"/>
   </bookViews>
@@ -73,15 +73,6 @@
     <t>NNOutput</t>
   </si>
   <si>
-    <t>x_axis</t>
-  </si>
-  <si>
-    <t>y_axis</t>
-  </si>
-  <si>
-    <t>z_axis</t>
-  </si>
-  <si>
     <t>MSE</t>
   </si>
   <si>
@@ -101,6 +92,15 @@
   </si>
   <si>
     <t>newOutput</t>
+  </si>
+  <si>
+    <t>x_axis</t>
+  </si>
+  <si>
+    <t>y_axis</t>
+  </si>
+  <si>
+    <t>z_axis</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:P2001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +464,8 @@
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="6" customWidth="1"/>
+    <col min="5" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
@@ -487,13 +488,13 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -502,25 +503,25 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>